<commit_message>
Separate upload folders and sample data
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data - Looking Glass.xlsx
+++ b/Documentation/Sample Data - Looking Glass.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\incin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\incin\Desktop\looking-glass\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46FF85A9-1B68-4D6D-8A48-9D54357A41C3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92132B2-D09D-485C-A01E-7F09D1E98A3C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{C0B7F08B-A843-48E2-96EF-753B93976E9F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -40,6 +40,138 @@
   </si>
   <si>
     <t>Images (filename)</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Sadhwani</t>
+  </si>
+  <si>
+    <t>stevo</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Hafer</t>
+  </si>
+  <si>
+    <t>pauleatstoomuch</t>
+  </si>
+  <si>
+    <t>paul</t>
+  </si>
+  <si>
+    <t>Zack</t>
+  </si>
+  <si>
+    <t>Wakeley</t>
+  </si>
+  <si>
+    <t>zackman40</t>
+  </si>
+  <si>
+    <t>zack</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Fuentes</t>
+  </si>
+  <si>
+    <t>mikey</t>
+  </si>
+  <si>
+    <t>mike</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Barker</t>
+  </si>
+  <si>
+    <t>bobbyb</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Tindell</t>
+  </si>
+  <si>
+    <t>rtindell</t>
+  </si>
+  <si>
+    <t>ralph</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Finnegan</t>
+  </si>
+  <si>
+    <t>patrickf</t>
+  </si>
+  <si>
+    <t>patrick</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>maryf</t>
+  </si>
+  <si>
+    <t>mary</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>Merchant</t>
+  </si>
+  <si>
+    <t>joeym</t>
+  </si>
+  <si>
+    <t>joey</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Pennyworth</t>
+  </si>
+  <si>
+    <t>batman</t>
+  </si>
+  <si>
+    <t>masterbruce</t>
+  </si>
+  <si>
+    <t>ap1.jpg,ap2.jpg,ap3.jpg,ap4.jpg,ap5.jpg</t>
+  </si>
+  <si>
+    <t>bb1.jpg,bb2.jpg,bb3.jpg,bb4.jpg,bb5.jpg</t>
+  </si>
+  <si>
+    <t>jm1.jpg,jm2.jpg,jm3.jpg,jm4.jpg,jm5.jpg</t>
+  </si>
+  <si>
+    <t>mf1.jpg,mf2.jpg,mf3.jpg,mf4.jpg</t>
+  </si>
+  <si>
+    <t>pf1.jpg,pf2.jpg,pf3.jpg,pf4.jpg,pf5.jpg</t>
   </si>
 </sst>
 </file>
@@ -485,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4114E0A4-7A80-45E0-82C8-09ACC9C7EFAF}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,74 +648,164 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded Photos for each user, added all data to DB, and cleaned up repo
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data - Looking Glass.xlsx
+++ b/Documentation/Sample Data - Looking Glass.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\incin\Desktop\looking-glass\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Incinerator\Desktop\CIS 4930 - Advanced Python\looking-glass\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92132B2-D09D-485C-A01E-7F09D1E98A3C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715F3742-0AF4-42A1-B3C5-839754F6B7E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{C0B7F08B-A843-48E2-96EF-753B93976E9F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>First Name</t>
   </si>
@@ -159,19 +159,34 @@
     <t>masterbruce</t>
   </si>
   <si>
-    <t>ap1.jpg,ap2.jpg,ap3.jpg,ap4.jpg,ap5.jpg</t>
-  </si>
-  <si>
     <t>bb1.jpg,bb2.jpg,bb3.jpg,bb4.jpg,bb5.jpg</t>
   </si>
   <si>
     <t>jm1.jpg,jm2.jpg,jm3.jpg,jm4.jpg,jm5.jpg</t>
   </si>
   <si>
-    <t>mf1.jpg,mf2.jpg,mf3.jpg,mf4.jpg</t>
-  </si>
-  <si>
     <t>pf1.jpg,pf2.jpg,pf3.jpg,pf4.jpg,pf5.jpg</t>
+  </si>
+  <si>
+    <t>ap1.jpg,ap2.jpg,ap3.jpg,ap4.png,ap5.jpg</t>
+  </si>
+  <si>
+    <t>ss1.jpg,ss2.jpg,ss3.jpg,ss4.jpg,ss5.jpg</t>
+  </si>
+  <si>
+    <t>ph1.jpg,ph2,jpg,ph3,jpg,ph4.jpg,ph5.jpg</t>
+  </si>
+  <si>
+    <t>zw1.jpg,zw2.jpg,zw3.jpg,zw4.jpg,zw5.jpg</t>
+  </si>
+  <si>
+    <t>mf1.jpg,mf2.jpg,mf3.jpg,mf4.jpg,mf5.jpg</t>
+  </si>
+  <si>
+    <t>rt1.jpg,rt2.jpg,rt3.jpg,rt4.jpg,rt5.jpg</t>
+  </si>
+  <si>
+    <t>mff1.jpg,mff2.jpg,mff3.jpg,mff4.jpg,mff5.jpg</t>
   </si>
 </sst>
 </file>
@@ -617,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4114E0A4-7A80-45E0-82C8-09ACC9C7EFAF}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +675,9 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -675,7 +692,9 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -690,7 +709,9 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -706,7 +727,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -723,7 +744,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,7 +760,9 @@
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -755,7 +778,7 @@
         <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -771,7 +794,9 @@
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -787,7 +812,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -804,7 +829,7 @@
         <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>